<commit_message>
pcb: Add DWM1000 to its adapter assembly files
Add the DWM1000 module to the assembly files of the DWM1000 adapter
board.
</commit_message>
<xml_diff>
--- a/pcb/dwm1000_adapter/DecawaveProMiniAdapter_BOM_PCBWay.xlsx
+++ b/pcb/dwm1000_adapter/DecawaveProMiniAdapter_BOM_PCBWay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip\Downloads\decawave_pro_mini_adapter_wayne_holder_modified_by_filip_schauer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Android_NDK\AlphabotSZUCar\AlphabotSZUCar\pcb\dwm1000_adapter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9D2CB1-1A30-4302-8FDC-39D2F9C31CF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61006FF-2B8B-468D-A841-6B109D433850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4515" yWindow="4215" windowWidth="18585" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Item #</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>U1,U2,U3</t>
+  </si>
+  <si>
+    <t>DWM1000</t>
+  </si>
+  <si>
+    <t>Decawave</t>
+  </si>
+  <si>
+    <t>IC RF-Module UWB Transceiver</t>
   </si>
 </sst>
 </file>
@@ -728,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1011,6 +1020,31 @@
         <v>9</v>
       </c>
       <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="3">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="6"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="8"/>

</xml_diff>

<commit_message>
pcb: Add DWM1000 to its adapter assembly files (#10)
Add the DWM1000 module to the assembly files of the DWM1000 adapter
board.
</commit_message>
<xml_diff>
--- a/pcb/dwm1000_adapter/DecawaveProMiniAdapter_BOM_PCBWay.xlsx
+++ b/pcb/dwm1000_adapter/DecawaveProMiniAdapter_BOM_PCBWay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filip\Downloads\decawave_pro_mini_adapter_wayne_holder_modified_by_filip_schauer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Android_NDK\AlphabotSZUCar\AlphabotSZUCar\pcb\dwm1000_adapter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9D2CB1-1A30-4302-8FDC-39D2F9C31CF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F61006FF-2B8B-468D-A841-6B109D433850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4515" yWindow="4215" windowWidth="18585" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Item #</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>U1,U2,U3</t>
+  </si>
+  <si>
+    <t>DWM1000</t>
+  </si>
+  <si>
+    <t>Decawave</t>
+  </si>
+  <si>
+    <t>IC RF-Module UWB Transceiver</t>
   </si>
 </sst>
 </file>
@@ -728,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1011,6 +1020,31 @@
         <v>9</v>
       </c>
       <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="3">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="6"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="8"/>

</xml_diff>